<commit_message>
finished building basic UI and implemented abiliy to solve cube using CFOP
</commit_message>
<xml_diff>
--- a/src/cfop/analysis.xlsx
+++ b/src/cfop/analysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="165">
   <si>
     <t>cross moves</t>
     <phoneticPr fontId="1"/>
@@ -108,67 +108,515 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>R' B U' L2 R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 L F' L F L' U L' U L' U L U L' U' L F' U' F U2 F' U F U R' F R U R' U' F' R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 R' F' L F' L' F2 R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' B U' L2 R U2 L F' L F L' U L' U L' U L U L' U' L F' U' F U2 F' U F U R' F R U R' U' F' R U2 R' F' L F' L' F2 R M2 U M' U2 M U M2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R U B2 L D' R' U' B R U F2 B2 U' R2 D' R2 F2 U' L2 B2 U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' F' U2 F' L</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' F R' F' R U' R U R' U L' U' L' U' L' U L U L U' R' F' U2 F R U2 L' U L U' F U F'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U L F L' R U R' U' L F' L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R' U R' U' R D' R' D R' U D' R2 U' R2 D R2 U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' F' U2 F' L U' F R' F' R U' R U R' U L' U' L' U' L' U L U L U' R' F' U2 F R U2 L' U L U' F U F' U L F L' R U R' U' L F' L' U R' U R' U' R D' R' D R' U D' R2 U' R2 D R2 U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B U2 L' B L2 U' B2 U' F L U2 R2 D F2 U' L2 D R2 F2 B2 U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R F' D L' D F2 R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R U' R' U' R U' R' U R U' R' F U' F' U2 L' U' L L U' L' U2 R' U F' U F R U' R' U R U2 L U2 L' U' L U L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R U B' U' R' U R B R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' U L' U2 R U' L R' U L' U2 R U' L U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R F' D L' D F2 U' R' U' R U' R' U R U' R' F U' F' U2 L' U' L2 U' L' U2 R' U F' U F R U' R' U R U2 L U2 L' U' L U L' U R U B' U' R' U R B R2 U L' U2 R U' L R' U L' U2 R U' L U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B2 R U' B D F2 R2 D' L F R2 F2 D2 L2 U2 R2 B D2 F B2 R2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L' D' B L D L' B'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L' U2 L U L' U' L U L F' L' U' L U F L' U R U2 R' U F' U' F U' R' U F' U F R U' R' U R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' B' R B U B' U' R' U B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U M2 U M' U2 M U M2 U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L' D' B L D L' B' L' U2 L U L' U' L U L F' L' U' L U F L' U R U2 R' U F' U' F U' R' U F' U F R U' R' U R U' B' R B U B' U' R' U B U M2 U M' U2 M U M2 U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D' L2 U L D' B' D F2 L' R2 D B2 U2 F2 R2 U' R2 D2 F2 U' F2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D U' R2 D R F' R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U L' U' L' U' L' U L U L U2 R U2 R' U' R U R' U' F R U R2 U' R F' U2 L' U2 L U L' U2 L</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' F' L F L' U2 F2 R' F' R F'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' R U R' F' U' F R U R' F R' F' R2 U2 R' U'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D U' R2 D R F' R U L' U' L' U' L' U L U L U2 R U2 R' U' R U R' U' F R U R2 U' R F' U2 L' U2 L U L' U2 L U' F' L F L' U2 F2 R' F' R F' U' R U R' F' U' F R U R' F R' F' R2 U2 R' U'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R U L2 F D2 F L U' L2 F' B' L2 B U2 B' U2 R2 U2 F2 R D</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' D' R' L B L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R U2 R2 F R F' U2 R' B' U' R U R' B U R L' U' L2 U' L' U2 L U L' U L U' L' U2 F U' F'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>M2 U M' U2 M U M2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' D' R' L B L' U R U2 R2 F R F' U2 R' B' U' R U R' B U R L' U' L2 U' L' U2 L U L' U L U' L' U2 F U' F' R U R' U R U' R' U R U2 R' M2 U M' U2 M U M2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B' L' R2 U B2 R2 U' R2 F2 D2 R2 L' F R2 F' D B D</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' R B' D U' F2 R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 L U L' U L U' L' U' R' U R U2 R' F L F' L' F' R R U R' U R' F R F'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U F' U2 F' L F L' U' L' U' L U' F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R U R' F' U' F R U R' F R' F' R2 U2 R' U'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' R B' D U' F2 R' U2 L U L' U L U' L' U' R' U R U2 R' F L F' L' F' R2 U R' U R' F R F' U F' U2 F' L F L' U' L' U' L U' F R U R' F' U' F R U R' F R' F' R2 U2 R' U'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L R U D B L R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D R' B D' R' B' L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' U2 R2 U R2 U R U L U' L F' L' F L' L' U' L R' U2 R U2 R' U R U2 L' U' L U L' U' L</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 R U R' U R U' B U' B' R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' R U R' U' D R2 U' R U' R' U R' U R2 D' U'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D R' B D' R' B' L' R' U2 R2 U R2 U R U L U' L F' L' F L2 U' L R' U2 R U2 R' U R U2 L' U' L U L' U' L U2 R U R' U R U' B U' B' R' U' R U R' U' D R2 U' R U' R' U R' U R2 D' U'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L2 U R U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R' L2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R U R' F U' R U R' U F'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' F R U R' U' F2 L' U' L U F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 R' U' F' R U R' U' R' F R2 U' R' U' R U R' U R U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R' L2 R U R' F U' R U R' U F' U' F R U R' U' F2 L' U' L U F U2 R' U' F' R U R' U' R' F R2 U' R' U' R U R' U R U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R L' U' D L2 B2 D2 L' U L2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L' D U B2 R' L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L' U' L U' R' B' U' R U R' B U R U2 F2 R U R' U' F2 U' L U L' U L U' L' R U2 R' U R' F R F'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>F R U R' U' F2 L' U' L U F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R U R' U' R' F R2 U' R' U' R U R' F' U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L' D U B2 R' L2 U' L U' R' B' U' R U R' B U R U2 F2 R U R' U' F2 U' L U L' U L U' L' R U2 R' U R' F R R U R' U' F2 L' U' L U F R U R' U' R' F R2 U' R' U' R U R' F' U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B2 F U F' L' D B2 R2 D L2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R F2 L' R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 R U R' U2 R U R2 U R U' R' U R U2 R' U R U L F R U' R' F' L' U' L' U2 L U' F U F'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' R' U2 F R U R' U' F2 U2 F R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 R' U2 R U2 R' F R U R' U' R' F' R2 U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R F2 L' R U2 R U R' U2 R U R2 U R U' R' U R U2 R' U R U L F R U' R' F' L' U' L' U2 L U' F U F' U' R' U2 F R U R' U' F2 U2 F R U2 R' U2 R U2 R' F R U R' U' R' F' R2 U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' L U D U' L' B' U2 B2 F'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L' B' D' L B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 F R2 U R2 U' R2 F' U2 R U' R' F R' F' R U L U' L' U' F' U' L' U L F L' U L2 F R U' R' F' L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' R U R' U R U' B U' B' R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' U R' U' R D' R' D R' U D' R2 U' R2 D R2 U'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L' B' D' L B U2 F R2 U R2 U' R2 F' U2 R U' R' F R' F' R U L U' L' U' F' U' L' U L F L' U L2 F R U' R' F' L' U' R U R' U R U' B U' B' R2 U R' U' R D' R' D R' U D' R2 U' R2 D R2 U'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B' U D' R2 L F' B2 F B U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B D R U' B' R' F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L2 U2 F' L2 F U2 L U' L R U R' R U R' U2 R' U2 R U R' U' R U2 R U2 R2 F R F' U2 L U L' U2 L U L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L F L' R U R' U' L F' L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' U L' U2 R U' L R' U L' U2 R U' L U</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B D R U' B' R' F L2 U2 F' L2 F U2 L U' L R U U R' U2 R' U2 R U R' U' R U2 R U2 R2 F R F' U2 L U L' U2 L U F L' R U R' U' L F' L' R' U L' U2 R U' L R' U L' U2 R U' L U</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B F B D2 R' F U2 L D' B2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>F2 D2 L' R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U L F' L' F L' U' L U2 L F U F2 L F L2 U R U R' U2 R' F' U2 F R U' R U R' U R U' R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R U R' U R U' R' U R U2 R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' R' U' R U D' R2 U R' U R U' R U' R2 D U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>F2 D2 L' R U L F' L' F L' U' L U2 L F U F2 L F L2 U R U R' U2 R' F' U2 F R U' R U R' U R U' U R' U R U' R' U R U2 R' U' R' U' R U D' R2 U R' U R U' R U' R2 D U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B F' R B F U D' R2 U F'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' D L F' L' R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>F R' F' R U' R U R' L U' L' U2 R' B' U' R U R' B U R U' F U R U2 R' U F' U2 F' L' U' L2 U L' F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R U2 R2 U' R2 U' R2 U2 R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R U R' U' D R2 U' R U' R' U R' U R2 D' U'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' D L F' L' R' F R' F' R U' R U R' L U' L' U2 R' B' U' R U R' B U R U' F U R U2 R' U F' U2 F' L' U' L2 U L' F U R U2 R2 U' R2 U' R2 U2 R U R U R' U' D R2 U' R U' R' U R' U R2 D' U'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L R2 D B' F2 L U' D R2 F2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R' D' B D' L' R' B'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U B U' B' U R U' R' U2 F U' F' U F U F' U' L U' L' U B' U' B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' L F L' R U R' U' L F' L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' R U2 R' U' R U2 L' U R' U' L U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R' D' B D' L' R' B' U B U' B' U R U' R' U2 F U' F' U F U F' U' L U' L' U B' U' B U' L F L' R U R' U' L F' L' U' R U2 R' U' R U2 L' U R' U' L U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>R2 F R B D R F2 L F' D2 L U2 R B2 R2 F2 R2 U2 R' D2 L2</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>R' B U' L2 R</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U2 L F' L F L' U L' U L' U L U L' U' L F' U' F U2 F' U F U R' F R U R' U' F' R</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U2 R' F' L F' L' F2 R</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>M2 U M' U2 M U M2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R' B U' L2 R U2 L F' L F L' U L' U L' U L U L' U' L F' U' F U2 F' U F U R' F R U R' U' F' R U2 R' F' L F' L' F2 R M2 U M' U2 M U M2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R U B2 L D' R' U' B R U F2 B2 U' R2 D' R2 F2 U' L2 B2 U2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R' F' U2 F' L</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U' F R' F' R U' R U R' U L' U' L' U' L' U L U L U' R' F' U2 F R U2 L' U L U' F U F'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U L F L' R U R' U' L F' L'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U R' U R' U' R D' R' D R' U D' R2 U' R2 D R2 U2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R' F' U2 F' L U' F R' F' R U' R U R' U L' U' L' U' L' U L U L U' R' F' U2 F R U2 L' U L U' F U F' U L F L' R U R' U' L F' L' U R' U R' U' R D' R' D R' U D' R2 U' R2 D R2 U2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>B U2 L' B L2 U' B2 U' F L U2 R2 D F2 U' L2 D R2 F2 B2 U2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R F' D L' D F2 R'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R U' R' U' R U' R' U R U' R' F U' F' U2 L' U' L L U' L' U2 R' U F' U F R U' R' U R U2 L U2 L' U' L U L'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U R U B' U' R' U R B R'</t>
+    <t>L2 D' B' L' B D' F2 L2 U2 F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B' D B' L' R F R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' R U' R' U2 R U' R' F' L F L' U' L' U' L U' L F U2 F' L' U' L U L' U B U' B'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L F L' U R U' R' U R U' R' L F' L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R2 B2 R F R' B2 R F' R U</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B' D B' L' R F R U' R U' R' U2 R U' R' F' L F L' U' L' U' L U' L F U2 F' L' U' L U L' U B U' B' L F L' U R U' R' U R U' R' L F' L' R2 B2 R F R' B2 R F' R U</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R U2 L' U F' D2 F2 U2 D' FU' D2 L2 B F L U B2 U' L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R B F D F L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R U R' L' U' U' L U L' U' L R' U2 F R U R' U' F' R L U' L' U2 R U2 R' U F' U' F U L U' L F' L2 U' L U F U L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R' F' L F' L' F2 R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' U2 R U2 R' F R U R' U' R' F' R2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R B F D F L' R U R' L' U2 L U L' U' L R' U2 F R U R' U' F' R L U' L' U2 R U2 R' U F' U' F U L U' L F' L2 U' L U F U L' U R' F' L F' L' F2 U2 R U2 R' F R U R' U' R' F' R2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D' L F' L F' B2 D2 B' R F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' R F D' U F R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U L' U' L U2 R' F R U R' U' F' R U R U2 R' U F' U' F U F U2 R U R' U F'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L F R' F' L' F R F'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 R U R' F' U' F R U R' F R' F' R2 U2 R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' R F D' U F R' U L' U' L U2 R' F R U R' U' F' R U R U2 R' U F' U' F U F U2 R U R' U F' L F R' F' L' F R F' U2 R U R' F' U' F R U R' F R' F' R2 U2 R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>F B2 R2 L' F' L' R2 B' F D</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B' L R2 U' F R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' L' U L F' L F L' U2 L U' L' U L U' L' U' F' U2 F U F' U' F U' R' F' U2 F R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U B' R B U B' U' R' U B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 R U' L' U R' U2 L U' L' U2 L U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B' L R2 U' F R' U' L' U L F' L F L' U2 L U' L' U L U' L' U' F' U2 F U F' U' F U' R' F' U2 F R U B' R B U B' U' R' U B U2 R U' L' U R' U2 L U' L' U2 L U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B2 L R2 L B D2 F2 D' R' L</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L' B L2 U R' F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 L U L' U2 L U L' F U F' R D R' U R D' R' U F R' F' R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U R' U' R' F R F' U R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R U R' U' D R2 U' R U' R' U R' U R2 D'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L' B L2 U R' F U2 L U L' U2 L U L' F U F' R D R' U R D' R' U F R' F' R U R' U' R' F R F' U R2 U R' U' D R2 U' R U' R' U R' U R2 D'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D2 R L' U B' R' U' L U2 B2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D2 R' F R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 R U R' U R U' R' F' L F L' U' L' U' L L U' L' R' U R U' R' U' R U' L F U F' L' U L U L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' F R U R' U' F'</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -176,151 +624,55 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>R F' D L' D F2 U' R' U' R U' R' U R U' R' F U' F' U2 L' U' L2 U' L' U2 R' U F' U F R U' R' U R U2 L U2 L' U' L U L' U R U B' U' R' U R B R2 U L' U2 R U' L R' U L' U2 R U' L U2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>B2 R U' B D F2 R2 D' L F R2 F2 D2 L2 U2 R2 B D2 F B2 R2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>L' D' B L D L' B'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>L' U2 L U L' U' L U L F' L' U' L U F L' U R U2 R' U F' U' F U' R' U F' U F R U' R' U R</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U' B' R B U B' U' R' U B</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U M2 U M' U2 M U M2 U2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>L' D' B L D L' B' L' U2 L U L' U' L U L F' L' U' L U F L' U R U2 R' U F' U' F U' R' U F' U F R U' R' U R U' B' R B U B' U' R' U B U M2 U M' U2 M U M2 U2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>D' L2 U L D' B' D F2 L' R2 D B2 U2 F2 R2 U' R2 D2 F2 U' F2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>D U' R2 D R F' R</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U L' U' L' U' L' U L U L U2 R U2 R' U' R U R' U' F R U R2 U' R F' U2 L' U2 L U L' U2 L</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U' F' L F L' U2 F2 R' F' R F'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U' R U R' F' U' F R U R' F R' F' R2 U2 R' U'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>D U' R2 D R F' R U L' U' L' U' L' U L U L U2 R U2 R' U' R U R' U' F R U R2 U' R F' U2 L' U2 L U L' U2 L U' F' L F L' U2 F2 R' F' R F' U' R U R' F' U' F R U R' F R' F' R2 U2 R' U'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R U L2 F D2 F L U' L2 F' B' L2 B U2 B' U2 R2 U2 F2 R D</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R' D' R' L B L'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U R U2 R2 F R F' U2 R' B' U' R U R' B U R L' U' L2 U' L' U2 L U L' U L U' L' U2 F U' F'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R U R' U R U' R' U R U2 R'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>M2 U M' U2 M U M2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R' D' R' L B L' U R U2 R2 F R F' U2 R' B' U' R U R' B U R L' U' L2 U' L' U2 L U L' U L U' L' U2 F U' F' R U R' U R U' R' U R U2 R' M2 U M' U2 M U M2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>B' L' R2 U B2 R2 U' R2 F2 D2 R2 L' F R2 F' D B D</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U' R B' D U' F2 R'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U2 L U L' U L U' L' U' R' U R U2 R' F L F' L' F' R R U R' U R' F R F'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U F' U2 F' L F L' U' L' U' L U' F</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R U R' F' U' F R U R' F R' F' R2 U2 R' U'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U' R B' D U' F2 R' U2 L U L' U L U' L' U' R' U R U2 R' F L F' L' F' R2 U R' U R' F R F' U F' U2 F' L F L' U' L' U' L U' F R U R' F' U' F R U R' F R' F' R2 U2 R' U'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>L R U D B L R</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>D R' B D' R' B' L'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R' U2 R2 U R2 U R U L U' L F' L' F L' L' U' L R' U2 R U2 R' U R U2 L' U' L U L' U' L</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U2 R U R' U R U' B U' B' R'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U' R U R' U' D R2 U' R U' R' U R' U R2 D' U'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>D R' B D' R' B' L' R' U2 R2 U R2 U R U L U' L F' L' F L2 U' L R' U2 R U2 R' U R U2 L' U' L U L' U' L U2 R U R' U R U' B U' B' R' U' R U R' U' D R2 U' R U' R' U R' U R2 D' U'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>L2 U R U2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U R' L2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>R U R' F U' R U R' U F'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U' F R U R' U' F2 L' U' L U F</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U2 R' U' F' R U R' U' R' F R2 U' R' U' R U R' U R U2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>U R' L2 R U R' F U' R U R' U F' U' F R U R' U' F2 L' U' L U F U2 R' U' F' R U R' U' R' F R2 U' R' U' R U R' U R U2</t>
+    <t>D2 R' F R U2 R U R' U R U' R' F' L F L' U' L' U' L2 U' L' R' U R U' R' U' R U' L F U F' L' U L U L' U' F R U R' U' F' R' U L' U2 R U' L R' U L' U2 R U' L U2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R' U F L U2 F' B2 R D' B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B' D' B2 R F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>F U' R U R' U F' L U L' U' L U L' U' L U L' U2 R U' B U' B' U2 R U' F' U F R2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 F R U R' U' R U R' U' F'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 R' U2 R U2 R' F R U R' U' R' F' R2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B' D' B2 R F2 U' R U R' U F' L U L' U' L U L' U' L U L' U2 R U' B U' B' U2 R U' F' U F R2 U2 F R U R' U' R U R' U' F' U2 R' U2 R U2 R' F R U R' U' R' F' R2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>F D' U' F2 B U L' F' R2 L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D' F D' U' F B2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U2 R' U F' U F R U' R' U R U' R U R' U R' F R F' L U' L' U2 F U' F' U F U F' U' L U' L F' L2 U' L U F U L'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R U2 R2 F R F' R U2 R'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>U' R U R' F' U' F R U R' F R' F' R2 U2 R' U</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D' F D' U' F B2 U2 R' U F' U F R U' R' U R U' R U R' U R' F R F' L U' L' U2 F U' F' U F U F' U' L U' L F' L2 U' L U F U L' R U2 R2 F R F' R U2 R' U' R U R' F' U' F R U R' F R' F' R2 U2 R' U</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -659,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -739,7 +1091,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="">
+    <row r="2" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -792,15 +1144,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="">
+    <row r="3" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="B3">
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -809,7 +1161,7 @@
         <v>143</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3">
         <v>32</v>
@@ -818,7 +1170,7 @@
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3">
         <v>8</v>
@@ -827,7 +1179,7 @@
         <v>3</v>
       </c>
       <c r="L3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M3">
         <v>7</v>
@@ -836,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P3">
         <v>52</v>
@@ -845,15 +1197,15 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="">
+    <row r="4" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -862,7 +1214,7 @@
         <v>409</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4">
         <v>33</v>
@@ -871,7 +1223,7 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J4">
         <v>11</v>
@@ -880,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M4">
         <v>18</v>
@@ -889,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P4">
         <v>67</v>
@@ -898,15 +1250,15 @@
         <v>415</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="">
+    <row r="5" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>7</v>
@@ -915,7 +1267,7 @@
         <v>1583</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G5">
         <v>40</v>
@@ -924,7 +1276,7 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J5">
         <v>10</v>
@@ -933,7 +1285,7 @@
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>39</v>
+        <v>151</v>
       </c>
       <c r="M5">
         <v>15</v>
@@ -942,7 +1294,7 @@
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P5">
         <v>68</v>
@@ -951,15 +1303,15 @@
         <v>1589</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="">
+    <row r="6" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <v>7</v>
@@ -968,7 +1320,7 @@
         <v>8699</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G6">
         <v>35</v>
@@ -977,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J6">
         <v>10</v>
@@ -986,7 +1338,7 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M6">
         <v>9</v>
@@ -995,7 +1347,7 @@
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P6">
         <v>61</v>
@@ -1004,15 +1356,15 @@
         <v>8704</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="">
+    <row r="7" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -1021,7 +1373,7 @@
         <v>5605</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G7">
         <v>34</v>
@@ -1030,7 +1382,7 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J7">
         <v>11</v>
@@ -1039,7 +1391,7 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M7">
         <v>17</v>
@@ -1048,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P7">
         <v>69</v>
@@ -1057,15 +1409,15 @@
         <v>5610</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="">
+    <row r="8" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1074,7 +1426,7 @@
         <v>125</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G8">
         <v>34</v>
@@ -1083,7 +1435,7 @@
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="J8">
         <v>11</v>
@@ -1092,7 +1444,7 @@
         <v>2</v>
       </c>
       <c r="L8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M8">
         <v>7</v>
@@ -1101,7 +1453,7 @@
         <v>2</v>
       </c>
       <c r="O8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="P8">
         <v>58</v>
@@ -1110,15 +1462,15 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="">
+    <row r="9" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B9">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1127,7 +1479,7 @@
         <v>1694</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G9">
         <v>28</v>
@@ -1136,7 +1488,7 @@
         <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J9">
         <v>13</v>
@@ -1145,7 +1497,7 @@
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M9">
         <v>16</v>
@@ -1154,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="P9">
         <v>63</v>
@@ -1163,15 +1515,15 @@
         <v>1698</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="">
+    <row r="10" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B10">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -1180,7 +1532,7 @@
         <v>584</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G10">
         <v>33</v>
@@ -1189,7 +1541,7 @@
         <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J10">
         <v>11</v>
@@ -1198,7 +1550,7 @@
         <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M10">
         <v>17</v>
@@ -1207,7 +1559,7 @@
         <v>1</v>
       </c>
       <c r="O10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="P10">
         <v>67</v>
@@ -1216,15 +1568,15 @@
         <v>592</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="">
+    <row r="11" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -1233,7 +1585,7 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G11">
         <v>10</v>
@@ -1242,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J11">
         <v>12</v>
@@ -1251,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M11">
         <v>20</v>
@@ -1260,13 +1612,808 @@
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P11">
         <v>45</v>
       </c>
       <c r="Q11">
         <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>139</v>
+      </c>
+      <c r="F12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12">
+        <v>36</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12">
+        <v>11</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M12">
+        <v>15</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>79</v>
+      </c>
+      <c r="P12">
+        <v>65</v>
+      </c>
+      <c r="Q12">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13">
+        <v>34</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>84</v>
+      </c>
+      <c r="M13">
+        <v>15</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>85</v>
+      </c>
+      <c r="P13">
+        <v>66</v>
+      </c>
+      <c r="Q13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14">
+        <v>36</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>89</v>
+      </c>
+      <c r="J14">
+        <v>11</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>90</v>
+      </c>
+      <c r="M14">
+        <v>17</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>91</v>
+      </c>
+      <c r="P14">
+        <v>68</v>
+      </c>
+      <c r="Q14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15">
+        <v>38</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>96</v>
+      </c>
+      <c r="M15">
+        <v>15</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>97</v>
+      </c>
+      <c r="P15">
+        <v>66</v>
+      </c>
+      <c r="Q15">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>236</v>
+      </c>
+      <c r="F16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16">
+        <v>34</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>101</v>
+      </c>
+      <c r="J16">
+        <v>11</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>102</v>
+      </c>
+      <c r="M16">
+        <v>17</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>103</v>
+      </c>
+      <c r="P16">
+        <v>64</v>
+      </c>
+      <c r="Q16">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17">
+        <v>37</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>108</v>
+      </c>
+      <c r="M17">
+        <v>17</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>109</v>
+      </c>
+      <c r="P17">
+        <v>70</v>
+      </c>
+      <c r="Q17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>475</v>
+      </c>
+      <c r="F18" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18">
+        <v>24</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>113</v>
+      </c>
+      <c r="J18">
+        <v>11</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>114</v>
+      </c>
+      <c r="M18">
+        <v>13</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>115</v>
+      </c>
+      <c r="P18">
+        <v>56</v>
+      </c>
+      <c r="Q18">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="">
+      <c r="A19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>54</v>
+      </c>
+      <c r="F19" t="s">
+        <v>119</v>
+      </c>
+      <c r="G19">
+        <v>30</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19">
+        <v>14</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>121</v>
+      </c>
+      <c r="M19">
+        <v>10</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>122</v>
+      </c>
+      <c r="P19">
+        <v>61</v>
+      </c>
+      <c r="Q19">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="">
+      <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>93</v>
+      </c>
+      <c r="F20" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20">
+        <v>43</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>126</v>
+      </c>
+      <c r="J20">
+        <v>8</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>127</v>
+      </c>
+      <c r="M20">
+        <v>13</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>128</v>
+      </c>
+      <c r="P20">
+        <v>68</v>
+      </c>
+      <c r="Q20">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="">
+      <c r="A21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>170</v>
+      </c>
+      <c r="F21" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21">
+        <v>29</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>132</v>
+      </c>
+      <c r="J21">
+        <v>8</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>133</v>
+      </c>
+      <c r="M21">
+        <v>16</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
+        <v>134</v>
+      </c>
+      <c r="P21">
+        <v>60</v>
+      </c>
+      <c r="Q21">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="">
+      <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>52</v>
+      </c>
+      <c r="F22" t="s">
+        <v>137</v>
+      </c>
+      <c r="G22">
+        <v>30</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>138</v>
+      </c>
+      <c r="J22">
+        <v>10</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22" t="s">
+        <v>139</v>
+      </c>
+      <c r="M22">
+        <v>13</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>140</v>
+      </c>
+      <c r="P22">
+        <v>59</v>
+      </c>
+      <c r="Q22">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="">
+      <c r="A23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>89</v>
+      </c>
+      <c r="F23" t="s">
+        <v>143</v>
+      </c>
+      <c r="G23">
+        <v>23</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>144</v>
+      </c>
+      <c r="J23">
+        <v>9</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>145</v>
+      </c>
+      <c r="M23">
+        <v>15</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>146</v>
+      </c>
+      <c r="P23">
+        <v>52</v>
+      </c>
+      <c r="Q23">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="">
+      <c r="A24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G24">
+        <v>36</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>150</v>
+      </c>
+      <c r="J24">
+        <v>7</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>151</v>
+      </c>
+      <c r="M24">
+        <v>15</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
+        <v>152</v>
+      </c>
+      <c r="P24">
+        <v>61</v>
+      </c>
+      <c r="Q24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="">
+      <c r="A25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>155</v>
+      </c>
+      <c r="G25">
+        <v>31</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>156</v>
+      </c>
+      <c r="J25">
+        <v>11</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
+        <v>157</v>
+      </c>
+      <c r="M25">
+        <v>14</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25" t="s">
+        <v>158</v>
+      </c>
+      <c r="P25">
+        <v>60</v>
+      </c>
+      <c r="Q25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="">
+      <c r="A26" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>59</v>
+      </c>
+      <c r="F26" t="s">
+        <v>161</v>
+      </c>
+      <c r="G26">
+        <v>43</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>162</v>
+      </c>
+      <c r="J26">
+        <v>9</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26" t="s">
+        <v>163</v>
+      </c>
+      <c r="M26">
+        <v>17</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>164</v>
+      </c>
+      <c r="P26">
+        <v>75</v>
+      </c>
+      <c r="Q26">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>